<commit_message>
Update clustering and retrieval course material
</commit_message>
<xml_diff>
--- a/Machine Learning Specialisation (University of Washington)/4. Clustering and Retrieval/Quiz workings.xlsx
+++ b/Machine Learning Specialisation (University of Washington)/4. Clustering and Retrieval/Quiz workings.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\GitHub\Coursera\Machine Learning Specialisation (University of Washington)\4. Clustering and Retrieval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792FB90D-596F-48F8-9D65-76E3EBDA3A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59C8AF1-9190-4773-ADBE-B91F6A8DD0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{3A7B760A-3B31-4E27-9D85-3EF6FE5018AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{3A7B760A-3B31-4E27-9D85-3EF6FE5018AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="39">
   <si>
     <t>X1</t>
   </si>
@@ -126,6 +127,24 @@
   </si>
   <si>
     <t>Cluster responsibilities</t>
+  </si>
+  <si>
+    <t>Normalised</t>
+  </si>
+  <si>
+    <t>Unnormalised</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>alpha</t>
   </si>
 </sst>
 </file>
@@ -1296,6 +1315,153 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3E7C46E-4C46-4A5C-AF52-E34174587C18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2125980" cy="365760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B037C9D3-EA4E-44E2-9F29-F13EEF7BD366}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="365760"/>
+          <a:ext cx="2125980" cy="365760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2224,7 +2390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E064001-D86F-4304-BF31-A48D64D13146}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
@@ -2507,26 +2673,26 @@
         <v>2</v>
       </c>
       <c r="B14" s="3">
-        <f>$B2*B8</f>
+        <f t="shared" ref="B14:D16" si="0">$B2*B8</f>
         <v>0.60000000000000009</v>
       </c>
       <c r="C14" s="3">
-        <f>$B2*C8</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="D14" s="3">
-        <f>$B2*D8</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>20</v>
       </c>
       <c r="H14" s="5">
-        <f>$H2*H8</f>
+        <f t="shared" ref="H14:I16" si="1">$H2*H8</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="I14">
-        <f>$H2*I8</f>
+        <f t="shared" si="1"/>
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
@@ -2535,26 +2701,26 @@
         <v>3</v>
       </c>
       <c r="B15" s="3">
-        <f>$B3*B9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C15" s="3">
-        <f>$B3*C9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D15" s="3">
-        <f>$B3*D9</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>2</v>
       </c>
       <c r="H15">
-        <f>$H3*H9</f>
+        <f t="shared" si="1"/>
         <v>1.6240000000000001</v>
       </c>
       <c r="I15">
-        <f>$H3*I9</f>
+        <f t="shared" si="1"/>
         <v>0.81200000000000006</v>
       </c>
     </row>
@@ -2563,26 +2729,26 @@
         <v>4</v>
       </c>
       <c r="B16" s="3">
-        <f>$B4*B10</f>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
       <c r="C16" s="3">
-        <f>$B4*C10</f>
+        <f t="shared" si="0"/>
         <v>2.0999999999999996</v>
       </c>
       <c r="D16" s="3">
-        <f>$B4*D10</f>
+        <f t="shared" si="0"/>
         <v>4.8999999999999995</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H16">
-        <f>$H4*H10</f>
+        <f t="shared" si="1"/>
         <v>0.70200000000000007</v>
       </c>
       <c r="I16">
-        <f>$H4*I10</f>
+        <f t="shared" si="1"/>
         <v>1.6380000000000001</v>
       </c>
     </row>
@@ -2636,4 +2802,112 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0B85E5-5825-4042-8391-F50EB7B7C5A7}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f>3+G1</f>
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <f>20+G2</f>
+        <v>20.100000000000001</v>
+      </c>
+      <c r="D7">
+        <f>A7/A8*(B7/B8)</f>
+        <v>8.7802419354838707E-2</v>
+      </c>
+      <c r="E7">
+        <f>D7/SUM($D$7,$D$10)</f>
+        <v>0.55170885711495943</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f>5-1+(G3*G1)</f>
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <f>123+(G4*G2)</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f>1+G1</f>
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <f>36+G2</f>
+        <v>36.1</v>
+      </c>
+      <c r="D10">
+        <f>A10/A11*(B10/B11)</f>
+        <v>7.134387351778658E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f>4-1+(G3*G4)</f>
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <f>241+(G4*G2)</f>
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>